<commit_message>
Modify calc amount (by slippagee) method/ Add mainnet in config
</commit_message>
<xml_diff>
--- a/utils/outputData/performanceSummery.xlsx
+++ b/utils/outputData/performanceSummery.xlsx
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -66,6 +65,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -398,25 +465,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sat Apr 24 2021 23:35:56 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 01:22:53 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0xe83107dd13c7660dc56c15f69173d70fa99f924257fa9da577afd4e5efa741ff</t>
+          <t>0x03d76e2dcf30c4095f529d905add2df604b7823babc59270f28f7d5b316edfc9</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.000810897</t>
+          <t>0.000414524</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-0.000810897</v>
+        <v>0.01160065113598243</v>
       </c>
     </row>
     <row r="3">
@@ -428,23 +495,21 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sat Apr 24 2021 23:36:29 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 19:36:29 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0x3bfd672c5e4de1c2a5836c9166085d4f3f4a5f158f86ceb74c8c5919931ecc24</t>
+          <t>0x5e39157180c7266ddc648bc1ca7e735202e6ad42caa3f1aa381f4fcba7aef269</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.000644991</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0.017721227077105216</t>
-        </is>
+          <t>0.00041387</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.000425553863434797</v>
       </c>
     </row>
     <row r="4">
@@ -456,23 +521,21 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sat Apr 24 2021 23:36:57 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 20:18:25 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0x68b181735ff171febd9a9c137289f9cbb186c593574d2768ca0ba08e0a211315</t>
+          <t>0xf556f6ab7055d48f9ebc5cc3f5c3ef9fbd7f102c83510ec197a9b05ba96f3d07</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.000644991</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0.005366538662097504</t>
-        </is>
+          <t>0.000414568</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01053781198224355</v>
       </c>
     </row>
     <row r="5">
@@ -484,23 +547,21 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 13:42:57 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 20:40:21 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0xf10fd5889cb5274f6ffb03e94f85f80db926ee032495da9c196f3222e4ea2a5e</t>
+          <t>0x003e2e03654b5c888e9c9142fda0e61e178b5ee0acf3741c3a4f2f28cc0af6c1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.0002579964</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0.008817436828807392</t>
-        </is>
+          <t>0.000414568</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.009564243733416767</v>
       </c>
     </row>
     <row r="6">
@@ -512,23 +573,21 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 13:55:37 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 20:42:09 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0x98ba671b2d35bf9fc8b6459994dae9d3ca34e9ec45e966abfc0ac3a113c8883c</t>
+          <t>0xdecc9f5ea2d2027f5448db538b5ce52eeadf7531b48b7c3fde80ef8484420240</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.0002576376</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0.018927422847343512</t>
-        </is>
+          <t>0.000413894</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.02138397072097727</v>
       </c>
     </row>
     <row r="7">
@@ -540,23 +599,21 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 15:46:17 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 21:06:33 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0x88ffca512d3dbc01670abd33747523bdb7ddd13f163fc17e3857d1e71b4d1699</t>
+          <t>0x9dc151486cd3e88c6160f73c8f857ce59038e1e9bc8e4e25fcf8163eeff7e302</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.00214997</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0.11018031905369338</t>
-        </is>
+          <t>0.00041387</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.01939733196672238</v>
       </c>
     </row>
     <row r="8">
@@ -568,23 +625,21 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 15:46:44 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 21:08:32 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0x90f3b4fb284a6a68dfbcf3e2b6dddf10129728094a83def671c583f277a23e27</t>
+          <t>0x9dd2f6eed61bd4ffa60e782fefd9ee4ad8d8d80b68f29b15109c63647923e90c</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.00214997</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0.003450344884303968</t>
-        </is>
+          <t>0.000414568</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.005334091779495808</v>
       </c>
     </row>
     <row r="9">
@@ -596,23 +651,21 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 15:49:16 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 21:23:20 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0x631bf684f98930e18cbbc0c2551edb1812fd5f584a4f1903386a63e499db288f</t>
+          <t>0x583282fd9a2d74154237c30ac1a79fec24859322845f2a663c7f6f8b5d021cee</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.0021471</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.026410769264014961</t>
-        </is>
+          <t>0.000414568</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.008856762837462144</v>
       </c>
     </row>
     <row r="10">
@@ -624,23 +677,21 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 17:43:13 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 21:26:21 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0xe47fa0975b03848490c05beeea93466bce8298c3b60e595e9e4813d90a750b7b</t>
+          <t>0x6c77c8ba69d2e7b99323accffa81ce2cf9ab13096418bea81520d22f2aefc09b</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.00225329</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.23313926285894854</t>
-        </is>
+          <t>0.000413894</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.02233797328233905</v>
       </c>
     </row>
     <row r="11">
@@ -652,21 +703,21 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 17:52:21 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 21:32:30 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0xb5f4aea87101cc880c12b9d00ea67c200c97b41e85b88022752295fb9f1d1ed0</t>
+          <t>0xeb79ca09a138cc93c297e9a23787ffa6d418d22716a9c58267fdfe694f3bed8c</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.00225329</t>
+          <t>0.000414592</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.1525641123475137</v>
+        <v>-0.000246525737690668</v>
       </c>
     </row>
     <row r="12">
@@ -678,21 +729,21 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 18:12:32 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 21:32:49 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0x54ea526aef4e412d85430181f0c13133fa3cf433d5bd8ca84bcc9adcbdf0e82a</t>
+          <t>0xb91d2c95711ecba9bfd313e26b91554e0610810a7047ab27903db2b39d5d146f</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.00225317</t>
+          <t>0.000414592</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.0012533552692512</v>
+        <v>-0.000399706484896156</v>
       </c>
     </row>
     <row r="13">
@@ -704,21 +755,21 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 18:26:09 GMT+0900 (Japan Standard Time)</t>
+          <t>Mon Apr 26 2021 22:51:38 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0xd444cc110fac6b55e82fbc503a5ae4c1583d45bd2a394e846ff14c8d08fedb29</t>
+          <t>0xe3cc495009957ff54fa4b5b64d20573261f37879674605a7755b44d47c3a6c71</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.00045108</t>
+          <t>0.00621924</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-0.000255133215321819</v>
+        <v>-0.004770505782486944</v>
       </c>
     </row>
     <row r="14">
@@ -730,21 +781,177 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sun Apr 25 2021 18:31:32 GMT+0900 (Japan Standard Time)</t>
+          <t>Tue Apr 27 2021 00:03:52 GMT+0900 (Japan Standard Time)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0x14cd98fecfe9a5d2aa3f82d8c1d9c482dc7b663160ad5a609fce9d25e0a80f57</t>
+          <t>0x8d6fe5bd2e979f36208af5c4248484439efb4926b3dc78451e05db3fed362b04</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.000450634</t>
+          <t>0.001865772</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.007908697574910384</v>
+        <v>0.03646707030010118</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Tue Apr 27 2021 00:07:50 GMT+0900 (Japan Standard Time)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0x917829dc338fb8ae0cd3470699de86cfc32e136910ddfec3c62008137d55f1e8</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0.001862415</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.003592710552158496</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Tue Apr 27 2021 00:08:17 GMT+0900 (Japan Standard Time)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0x182529a4af3c89b41bc118885447dc687bd8c4a6a2f387c1c366caf5c88a00d7</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0.001862631</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001561784184273331</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Tue Apr 27 2021 00:34:57 GMT+0900 (Japan Standard Time)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0x738b3facd8c4b6cf6f5887f0666ee9b5a6ddead4d2866fc6436df050ea626311</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0.000620877</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.02332403784313836</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tue Apr 27 2021 00:35:53 GMT+0900 (Japan Standard Time)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0x4dc19f33d2e76a2407fc75d90a9133bcbee0c5f01859693c7d007e3231403b4f</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0.000787794</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.000787794</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Tue Apr 27 2021 00:36:29 GMT+0900 (Japan Standard Time)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0x2ccea5cf3fd393213296044bd37118b41735650c3c9f9a28fd6349edce05e3c3</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0.000621924</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.02639851150879546</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Tue Apr 27 2021 00:37:53 GMT+0900 (Japan Standard Time)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0x4891251aadf085682b5b207f7867d6896ca0dfbbefeb398af8d19a45d2674081</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.000621888</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0205843811667368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>